<commit_message>
Add result file conversion and condition file extraction
</commit_message>
<xml_diff>
--- a/diploma-backend/src/test/resources/file/conditions.xlsx
+++ b/diploma-backend/src/test/resources/file/conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PMerenkov\work\other\diploma\diploma-backend\src\main\resources\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projs\diploma\diploma-backend\src\test\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3133F10A-024A-46B8-B273-0F54DA5BA9AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F264C0F0-B0C8-4ED6-8135-7C3AE409A909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{CCE10A0D-518A-4DBC-A622-3155175D51BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CCE10A0D-518A-4DBC-A622-3155175D51BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Результат</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Сомнительно, но окей</t>
-  </si>
-  <si>
-    <t>Окей, но сомнительно</t>
   </si>
 </sst>
 </file>
@@ -80,7 +77,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -96,9 +93,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -136,7 +133,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -242,7 +239,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -392,34 +389,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4CADD9-65B2-46CB-A87C-41CCCBAFAFFB}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -427,54 +424,18 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>